<commit_message>
'Results from September_30,_2020--19:50:41 run'
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-09-30.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-09-30.xlsx
@@ -73,74 +73,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -521,47 +453,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C2" t="n">
-        <v>137564</v>
+        <v>293274</v>
       </c>
       <c r="D2" t="n">
-        <v>2399</v>
+        <v>8672</v>
       </c>
       <c r="E2" t="n">
-        <v>33938</v>
+        <v>39722</v>
       </c>
       <c r="F2" t="n">
-        <v>947</v>
+        <v>2226</v>
       </c>
       <c r="G2" t="n">
-        <v>36.57</v>
+        <v>13.54</v>
       </c>
       <c r="H2" t="n">
-        <v>41.01</v>
+        <v>25.67</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" t="n">
-        <v>92797</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2309</v>
-      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>1293186</v>
+        <v>1824125</v>
       </c>
       <c r="N2" t="n">
-        <v>26.58</v>
+        <v>14.23</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -572,29 +500,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44103</v>
+        <v>44104</v>
       </c>
       <c r="C3" t="n">
-        <v>5861</v>
+        <v>166033</v>
       </c>
       <c r="D3" t="n">
-        <v>56</v>
+        <v>5321</v>
       </c>
       <c r="E3" t="n">
-        <v>330</v>
+        <v>60522</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>2438</v>
       </c>
       <c r="G3" t="n">
-        <v>5.92</v>
+        <v>40.44</v>
       </c>
       <c r="H3" t="n">
-        <v>3.64</v>
+        <v>45.9</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -603,16 +531,16 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>5578</v>
+        <v>149649</v>
       </c>
       <c r="L3" t="n">
-        <v>55</v>
+        <v>5312</v>
       </c>
       <c r="M3" t="n">
-        <v>24129</v>
+        <v>1502916</v>
       </c>
       <c r="N3" t="n">
-        <v>3.27</v>
+        <v>32.23</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -623,29 +551,29 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C4" t="n">
-        <v>218507</v>
+        <v>87522</v>
       </c>
       <c r="D4" t="n">
-        <v>5650</v>
+        <v>2126</v>
       </c>
       <c r="E4" t="n">
-        <v>6652</v>
+        <v>3513</v>
       </c>
       <c r="F4" t="n">
-        <v>179</v>
+        <v>69</v>
       </c>
       <c r="G4" t="n">
-        <v>4.44</v>
+        <v>5.89</v>
       </c>
       <c r="H4" t="n">
-        <v>3.57</v>
+        <v>3.31</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -654,16 +582,16 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>149868</v>
+        <v>59598</v>
       </c>
       <c r="L4" t="n">
-        <v>5018</v>
+        <v>2087</v>
       </c>
       <c r="M4" t="n">
-        <v>305259</v>
+        <v>269854</v>
       </c>
       <c r="N4" t="n">
-        <v>4.39</v>
+        <v>3.7</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -674,200 +602,146 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Arkansas</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C5" t="n">
-        <v>82755</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1350</v>
-      </c>
-      <c r="E5" t="n">
-        <v>17369</v>
-      </c>
-      <c r="F5" t="n">
-        <v>264</v>
-      </c>
-      <c r="G5" t="n">
-        <v>23.52</v>
-      </c>
-      <c r="H5" t="n">
-        <v>21.85</v>
-      </c>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>73841</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1208</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
-        <v>460970</v>
+        <v>2179622</v>
       </c>
       <c r="N5" t="n">
-        <v>15.41</v>
+        <v>21.46</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>California</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>44103</v>
-      </c>
-      <c r="C6" t="n">
-        <v>810625</v>
-      </c>
-      <c r="D6" t="n">
-        <v>15792</v>
-      </c>
-      <c r="E6" t="n">
-        <v>24098</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1186</v>
-      </c>
-      <c r="G6" t="n">
-        <v>4.27</v>
-      </c>
-      <c r="H6" t="n">
-        <v>7.64</v>
-      </c>
+          <t>Wyoming</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
       </c>
-      <c r="K6" t="n">
-        <v>564767</v>
-      </c>
-      <c r="L6" t="n">
-        <v>15516</v>
-      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>2267875</v>
+        <v>5540</v>
       </c>
       <c r="N6" t="n">
-        <v>5.79</v>
+        <v>0.95</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>California - Los Angeles</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>44102</v>
-      </c>
-      <c r="C7" t="n">
-        <v>269284</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6551</v>
-      </c>
-      <c r="E7" t="n">
-        <v>7779</v>
-      </c>
-      <c r="F7" t="n">
-        <v>603</v>
-      </c>
-      <c r="G7" t="n">
-        <v>4.82</v>
-      </c>
-      <c r="H7" t="n">
-        <v>9.779999999999999</v>
-      </c>
+          <t>NewYork</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="b">
         <v>0</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
       </c>
-      <c r="K7" t="n">
-        <v>161332</v>
-      </c>
-      <c r="L7" t="n">
-        <v>6165</v>
-      </c>
-      <c r="M7" t="n">
-        <v>823987</v>
-      </c>
-      <c r="N7" t="n">
-        <v>8.16</v>
-      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
+          <t>New York -- New York</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44103</v>
-      </c>
-      <c r="C8" t="n">
-        <v>46985</v>
-      </c>
-      <c r="D8" t="n">
-        <v>781</v>
+        <v>44104</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>239219</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>19187</t>
+        </is>
       </c>
       <c r="E8" t="n">
-        <v>1715</v>
+        <v>37274</v>
       </c>
       <c r="F8" t="n">
-        <v>33</v>
+        <v>5345</v>
       </c>
       <c r="G8" t="n">
-        <v>4.41</v>
+        <v>27.99</v>
       </c>
       <c r="H8" t="n">
-        <v>4.25</v>
+        <v>30.39</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>38868</v>
+        <v>133172</v>
       </c>
       <c r="L8" t="n">
-        <v>777</v>
+        <v>17586</v>
       </c>
       <c r="M8" t="n">
-        <v>166412</v>
+        <v>2049418</v>
       </c>
       <c r="N8" t="n">
-        <v>5.04</v>
+        <v>24.27</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -878,58 +752,80 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>California - San Francisco</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44090</v>
+      </c>
+      <c r="C9" t="n">
+        <v>91304</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1220</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10190</v>
+      </c>
+      <c r="F9" t="n">
+        <v>229</v>
+      </c>
+      <c r="G9" t="n">
+        <v>12.28</v>
+      </c>
+      <c r="H9" t="n">
+        <v>19.07</v>
+      </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>82991</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1201</v>
+      </c>
+      <c r="M9" t="n">
+        <v>368744</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6.38</v>
+      </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Wisconsin -- Milwaukee</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44103</v>
+        <v>44104</v>
       </c>
       <c r="C10" t="n">
-        <v>70025</v>
+        <v>29054</v>
       </c>
       <c r="D10" t="n">
-        <v>2046</v>
+        <v>428</v>
       </c>
       <c r="E10" t="n">
-        <v>2927</v>
+        <v>7050</v>
       </c>
       <c r="F10" t="n">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="G10" t="n">
-        <v>5.03</v>
+        <v>25.84</v>
       </c>
       <c r="H10" t="n">
-        <v>6.42</v>
+        <v>35.98</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -938,16 +834,16 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>58149</v>
+        <v>27282</v>
       </c>
       <c r="L10" t="n">
-        <v>2008</v>
+        <v>428</v>
       </c>
       <c r="M10" t="n">
-        <v>227938</v>
+        <v>252321</v>
       </c>
       <c r="N10" t="n">
-        <v>4.12</v>
+        <v>26.44</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -958,32 +854,18 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Connecticut</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>44102</v>
-      </c>
-      <c r="C11" t="n">
-        <v>54919</v>
-      </c>
-      <c r="D11" t="n">
-        <v>3608</v>
-      </c>
-      <c r="E11" t="n">
-        <v>7413</v>
-      </c>
-      <c r="F11" t="n">
-        <v>662</v>
-      </c>
-      <c r="G11" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="H11" t="n">
-        <v>18.35</v>
-      </c>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -991,43 +873,43 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>378262</v>
+        <v>77789</v>
       </c>
       <c r="N11" t="n">
-        <v>10.56</v>
+        <v>1.91</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44104</v>
+        <v>44015</v>
       </c>
       <c r="C12" t="n">
-        <v>20613</v>
+        <v>16491</v>
       </c>
       <c r="D12" t="n">
-        <v>636</v>
+        <v>960</v>
       </c>
       <c r="E12" t="n">
-        <v>5451</v>
+        <v>1592</v>
       </c>
       <c r="F12" t="n">
-        <v>163</v>
+        <v>48</v>
       </c>
       <c r="G12" t="n">
-        <v>28.7</v>
+        <v>12.29</v>
       </c>
       <c r="H12" t="n">
-        <v>25.63</v>
+        <v>6.14</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -1036,16 +918,16 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>18990</v>
+        <v>12950</v>
       </c>
       <c r="L12" t="n">
-        <v>636</v>
+        <v>782</v>
       </c>
       <c r="M12" t="n">
-        <v>209892</v>
+        <v>69254</v>
       </c>
       <c r="N12" t="n">
-        <v>22.11</v>
+        <v>6.55</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1056,88 +938,72 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Florida</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C13" t="n">
-        <v>698051</v>
-      </c>
-      <c r="D13" t="n">
-        <v>14315</v>
-      </c>
-      <c r="E13" t="n">
-        <v>93993</v>
-      </c>
-      <c r="F13" t="n">
-        <v>2499</v>
-      </c>
-      <c r="G13" t="n">
-        <v>13.47</v>
-      </c>
-      <c r="H13" t="n">
-        <v>17.46</v>
-      </c>
+          <t>SouthCarolina</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>3316376</v>
-      </c>
-      <c r="N13" t="n">
-        <v>16.1</v>
-      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Florida -- Miami-Dade County</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C14" t="n">
-        <v>170400</v>
+        <v>196139</v>
       </c>
       <c r="D14" t="n">
-        <v>3280</v>
+        <v>2454</v>
       </c>
       <c r="E14" t="n">
-        <v>14995</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
+        <v>35639</v>
+      </c>
+      <c r="F14" t="n">
+        <v>667</v>
+      </c>
       <c r="G14" t="n">
-        <v>14.03</v>
-      </c>
-      <c r="H14" t="inlineStr"/>
+        <v>18.17</v>
+      </c>
+      <c r="H14" t="n">
+        <v>27.18</v>
+      </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="n">
-        <v>106890</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>481976</v>
+        <v>1117489</v>
       </c>
       <c r="N14" t="n">
-        <v>17.75</v>
+        <v>16.8</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1148,24 +1014,24 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Florida -- Orange County</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C15" t="n">
-        <v>40329</v>
+        <v>5390</v>
       </c>
       <c r="D15" t="n">
-        <v>458</v>
+        <v>141</v>
       </c>
       <c r="E15" t="n">
-        <v>6126</v>
+        <v>978</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>22.98</v>
+        <v>19.89</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="b">
@@ -1175,14 +1041,14 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>26656</v>
+        <v>4917</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>277193</v>
+        <v>17881</v>
       </c>
       <c r="N15" t="n">
-        <v>20.98</v>
+        <v>1.34</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1193,88 +1059,80 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Georgia</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C16" t="n">
-        <v>318026</v>
-      </c>
-      <c r="D16" t="n">
-        <v>7021</v>
-      </c>
-      <c r="E16" t="n">
-        <v>84015</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2881</v>
-      </c>
-      <c r="G16" t="n">
-        <v>26.42</v>
-      </c>
-      <c r="H16" t="n">
-        <v>41.03</v>
-      </c>
+          <t>Maryland</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>3239300</v>
+        <v>1788090</v>
       </c>
       <c r="N16" t="n">
-        <v>31.46</v>
+        <v>29.78</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hawaii</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44103</v>
+        <v>44104</v>
       </c>
       <c r="C17" t="n">
-        <v>12290</v>
+        <v>137564</v>
       </c>
       <c r="D17" t="n">
-        <v>134</v>
+        <v>2399</v>
       </c>
       <c r="E17" t="n">
-        <v>164</v>
-      </c>
-      <c r="F17" t="inlineStr"/>
+        <v>33938</v>
+      </c>
+      <c r="F17" t="n">
+        <v>947</v>
+      </c>
       <c r="G17" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H17" t="inlineStr"/>
+        <v>36.57</v>
+      </c>
+      <c r="H17" t="n">
+        <v>41.01</v>
+      </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>6573</v>
-      </c>
-      <c r="L17" t="inlineStr"/>
+        <v>92797</v>
+      </c>
+      <c r="L17" t="n">
+        <v>2309</v>
+      </c>
       <c r="M17" t="n">
-        <v>26266</v>
+        <v>1293186</v>
       </c>
       <c r="N17" t="n">
-        <v>1.85</v>
+        <v>26.58</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1285,65 +1143,69 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Idaho</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+          <t>Arkansas</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C18" t="n">
+        <v>83697</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1369</v>
+      </c>
+      <c r="E18" t="n">
+        <v>17527</v>
+      </c>
+      <c r="F18" t="n">
+        <v>268</v>
+      </c>
+      <c r="G18" t="n">
+        <v>23.44</v>
+      </c>
+      <c r="H18" t="n">
+        <v>21.84</v>
+      </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>74772</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1227</v>
+      </c>
       <c r="M18" t="n">
-        <v>11536</v>
+        <v>460970</v>
       </c>
       <c r="N18" t="n">
-        <v>0.68</v>
+        <v>15.41</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Illinois</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C19" t="n">
-        <v>293274</v>
-      </c>
-      <c r="D19" t="n">
-        <v>8672</v>
-      </c>
-      <c r="E19" t="n">
-        <v>39722</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2226</v>
-      </c>
-      <c r="G19" t="n">
-        <v>13.54</v>
-      </c>
-      <c r="H19" t="n">
-        <v>25.67</v>
-      </c>
+          <t>Ohio</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="b">
         <v>0</v>
@@ -1351,57 +1213,57 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>1824125</v>
+        <v>1438271</v>
       </c>
       <c r="N19" t="n">
-        <v>14.23</v>
+        <v>12.35</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44104</v>
+        <v>44103</v>
       </c>
       <c r="C20" t="n">
-        <v>120019</v>
+        <v>55129</v>
       </c>
       <c r="D20" t="n">
-        <v>3405</v>
+        <v>3610</v>
       </c>
       <c r="E20" t="n">
-        <v>11545</v>
+        <v>7418</v>
       </c>
       <c r="F20" t="n">
-        <v>449</v>
+        <v>662</v>
       </c>
       <c r="G20" t="n">
-        <v>9.619999999999999</v>
+        <v>13.46</v>
       </c>
       <c r="H20" t="n">
-        <v>13.19</v>
+        <v>18.34</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>619472</v>
+        <v>378262</v>
       </c>
       <c r="N20" t="n">
-        <v>9.33</v>
+        <v>10.56</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1412,43 +1274,43 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C21" t="n">
-        <v>88829</v>
+        <v>124615</v>
       </c>
       <c r="D21" t="n">
-        <v>1344</v>
+        <v>6704</v>
       </c>
       <c r="E21" t="n">
-        <v>5023</v>
+        <v>26155</v>
       </c>
       <c r="F21" t="n">
-        <v>52</v>
+        <v>2546</v>
       </c>
       <c r="G21" t="n">
-        <v>5.65</v>
+        <v>20.99</v>
       </c>
       <c r="H21" t="n">
-        <v>3.87</v>
+        <v>37.98</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>109911</v>
+        <v>1375424</v>
       </c>
       <c r="N21" t="n">
-        <v>3.51</v>
+        <v>13.81</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1459,7 +1321,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Hawaii</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1478,112 +1340,86 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>169801</v>
+        <v>26266</v>
       </c>
       <c r="N22" t="n">
-        <v>5.84</v>
+        <v>1.85</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Kentucky</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>44103</v>
-      </c>
-      <c r="C23" t="n">
-        <v>67856</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1170</v>
-      </c>
-      <c r="E23" t="n">
-        <v>5517</v>
-      </c>
-      <c r="F23" t="n">
-        <v>136</v>
-      </c>
-      <c r="G23" t="n">
-        <v>11.84</v>
-      </c>
-      <c r="H23" t="n">
-        <v>12.8</v>
-      </c>
+          <t>Oklahoma</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" t="n">
-        <v>46603</v>
-      </c>
-      <c r="L23" t="n">
-        <v>1069</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>354112</v>
+        <v>287959</v>
       </c>
       <c r="N23" t="n">
-        <v>7.98</v>
+        <v>7.35</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C24" t="n">
-        <v>166033</v>
+        <v>13071</v>
       </c>
       <c r="D24" t="n">
-        <v>5321</v>
+        <v>180</v>
       </c>
       <c r="E24" t="n">
-        <v>60522</v>
-      </c>
-      <c r="F24" t="n">
-        <v>2438</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
-        <v>40.44</v>
-      </c>
-      <c r="H24" t="n">
-        <v>45.9</v>
-      </c>
+        <v>0.57</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="b">
         <v>1</v>
       </c>
-      <c r="K24" t="n">
-        <v>149649</v>
-      </c>
-      <c r="L24" t="n">
-        <v>5312</v>
-      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
-        <v>1502916</v>
+        <v>4630</v>
       </c>
       <c r="N24" t="n">
-        <v>32.23</v>
+        <v>0.44</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1594,92 +1430,80 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Maine</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C25" t="n">
-        <v>5390</v>
-      </c>
-      <c r="D25" t="n">
-        <v>141</v>
-      </c>
-      <c r="E25" t="n">
-        <v>978</v>
-      </c>
+          <t>Kansas</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
-        <v>19.89</v>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" t="n">
-        <v>4917</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
-        <v>17881</v>
+        <v>169801</v>
       </c>
       <c r="N25" t="n">
-        <v>1.34</v>
+        <v>5.84</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C26" t="n">
-        <v>124725</v>
+        <v>6045</v>
       </c>
       <c r="D26" t="n">
-        <v>3805</v>
+        <v>56</v>
       </c>
       <c r="E26" t="n">
-        <v>39508</v>
+        <v>339</v>
       </c>
       <c r="F26" t="n">
-        <v>1558</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>37.31</v>
+        <v>5.87</v>
       </c>
       <c r="H26" t="n">
-        <v>41.06</v>
+        <v>3.64</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>105883</v>
+        <v>5772</v>
       </c>
       <c r="L26" t="n">
-        <v>3794</v>
+        <v>55</v>
       </c>
       <c r="M26" t="n">
-        <v>1788090</v>
+        <v>24129</v>
       </c>
       <c r="N26" t="n">
-        <v>29.78</v>
+        <v>3.27</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -1690,76 +1514,58 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>44103</v>
-      </c>
-      <c r="C27" t="n">
-        <v>131584</v>
-      </c>
-      <c r="D27" t="n">
-        <v>9423</v>
-      </c>
-      <c r="E27" t="n">
-        <v>12413</v>
-      </c>
-      <c r="F27" t="n">
-        <v>764</v>
-      </c>
-      <c r="G27" t="n">
-        <v>9.43</v>
-      </c>
-      <c r="H27" t="n">
-        <v>8.109999999999999</v>
-      </c>
+          <t>NorthDakota</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="b">
         <v>0</v>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
-      <c r="M27" t="n">
-        <v>510558</v>
-      </c>
-      <c r="N27" t="n">
-        <v>7.48</v>
-      </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'text'")</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C28" t="n">
-        <v>124615</v>
+        <v>132116</v>
       </c>
       <c r="D28" t="n">
-        <v>6704</v>
+        <v>9456</v>
       </c>
       <c r="E28" t="n">
-        <v>26155</v>
+        <v>12437</v>
       </c>
       <c r="F28" t="n">
-        <v>2546</v>
+        <v>766</v>
       </c>
       <c r="G28" t="n">
-        <v>20.99</v>
+        <v>9.41</v>
       </c>
       <c r="H28" t="n">
-        <v>37.98</v>
+        <v>8.1</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -1770,10 +1576,10 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>1375424</v>
+        <v>510558</v>
       </c>
       <c r="N28" t="n">
-        <v>13.81</v>
+        <v>7.48</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1784,43 +1590,41 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Florida -- Miami-Dade County</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C29" t="n">
-        <v>99134</v>
+        <v>170400</v>
       </c>
       <c r="D29" t="n">
-        <v>2036</v>
+        <v>3280</v>
       </c>
       <c r="E29" t="n">
-        <v>16920</v>
-      </c>
-      <c r="F29" t="n">
-        <v>195</v>
-      </c>
+        <v>14995</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>17.07</v>
-      </c>
-      <c r="H29" t="n">
-        <v>9.58</v>
-      </c>
+        <v>14.03</v>
+      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="b">
         <v>1</v>
       </c>
-      <c r="K29" t="inlineStr"/>
+      <c r="K29" t="n">
+        <v>106890</v>
+      </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
-        <v>342186</v>
+        <v>481976</v>
       </c>
       <c r="N29" t="n">
-        <v>6.19</v>
+        <v>17.75</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1831,43 +1635,41 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mississippi</t>
+          <t>Florida -- Orange County</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44103</v>
+        <v>44104</v>
       </c>
       <c r="C30" t="n">
-        <v>98190</v>
+        <v>40329</v>
       </c>
       <c r="D30" t="n">
-        <v>2969</v>
+        <v>458</v>
       </c>
       <c r="E30" t="n">
-        <v>38481</v>
-      </c>
-      <c r="F30" t="n">
-        <v>1373</v>
-      </c>
+        <v>6126</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
-        <v>39.19</v>
-      </c>
-      <c r="H30" t="n">
-        <v>46.24</v>
-      </c>
+        <v>22.98</v>
+      </c>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="b">
         <v>1</v>
       </c>
-      <c r="K30" t="inlineStr"/>
+      <c r="K30" t="n">
+        <v>26656</v>
+      </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
-        <v>1125834</v>
+        <v>277193</v>
       </c>
       <c r="N30" t="n">
-        <v>37.67</v>
+        <v>20.98</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -1878,90 +1680,80 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Missouri</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="n">
-        <v>44102</v>
-      </c>
-      <c r="C31" t="n">
-        <v>124620</v>
-      </c>
-      <c r="D31" t="n">
-        <v>2064</v>
-      </c>
-      <c r="E31" t="n">
-        <v>11641</v>
-      </c>
-      <c r="F31" t="n">
-        <v>496</v>
-      </c>
-      <c r="G31" t="n">
-        <v>26.42</v>
-      </c>
-      <c r="H31" t="n">
-        <v>31.9</v>
-      </c>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
       <c r="I31" t="b">
         <v>0</v>
       </c>
       <c r="J31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" t="n">
-        <v>44067</v>
-      </c>
-      <c r="L31" t="n">
-        <v>1555</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
       <c r="M31" t="n">
-        <v>704896</v>
+        <v>109911</v>
       </c>
       <c r="N31" t="n">
-        <v>11.57</v>
+        <v>3.51</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44104</v>
+        <v>44102</v>
       </c>
       <c r="C32" t="n">
-        <v>13071</v>
+        <v>124620</v>
       </c>
       <c r="D32" t="n">
-        <v>180</v>
+        <v>2064</v>
       </c>
       <c r="E32" t="n">
-        <v>75</v>
-      </c>
-      <c r="F32" t="inlineStr"/>
+        <v>11641</v>
+      </c>
+      <c r="F32" t="n">
+        <v>496</v>
+      </c>
       <c r="G32" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="H32" t="inlineStr"/>
+        <v>26.42</v>
+      </c>
+      <c r="H32" t="n">
+        <v>31.9</v>
+      </c>
       <c r="I32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="b">
         <v>1</v>
       </c>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
+      <c r="K32" t="n">
+        <v>44067</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1555</v>
+      </c>
       <c r="M32" t="n">
-        <v>4630</v>
+        <v>704896</v>
       </c>
       <c r="N32" t="n">
-        <v>0.44</v>
+        <v>11.57</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -1972,47 +1764,51 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44103</v>
-      </c>
-      <c r="C33" t="n">
-        <v>45044</v>
-      </c>
-      <c r="D33" t="n">
-        <v>478</v>
-      </c>
-      <c r="E33" t="n">
-        <v>2349</v>
-      </c>
-      <c r="F33" t="n">
-        <v>33</v>
+        <v>44104</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>73042</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>459</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>1473</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="G33" t="n">
-        <v>6.89</v>
+        <v>2</v>
       </c>
       <c r="H33" t="n">
-        <v>7.42</v>
+        <v>1.53</v>
       </c>
       <c r="I33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
-      </c>
-      <c r="K33" t="n">
-        <v>34087</v>
-      </c>
-      <c r="L33" t="n">
-        <v>445</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
       <c r="M33" t="n">
-        <v>90860</v>
+        <v>35862</v>
       </c>
       <c r="N33" t="n">
-        <v>4.77</v>
+        <v>1.18</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2023,47 +1819,43 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44104</v>
+        <v>44103</v>
       </c>
       <c r="C34" t="n">
-        <v>79980</v>
+        <v>98190</v>
       </c>
       <c r="D34" t="n">
-        <v>1600</v>
+        <v>2969</v>
       </c>
       <c r="E34" t="n">
-        <v>4964</v>
+        <v>38481</v>
       </c>
       <c r="F34" t="n">
-        <v>132</v>
+        <v>1373</v>
       </c>
       <c r="G34" t="n">
-        <v>8.300000000000001</v>
+        <v>39.19</v>
       </c>
       <c r="H34" t="n">
-        <v>12.26</v>
+        <v>46.24</v>
       </c>
       <c r="I34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="b">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
-        <v>59783</v>
-      </c>
-      <c r="L34" t="n">
-        <v>1077</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
-        <v>261123</v>
+        <v>1125834</v>
       </c>
       <c r="N34" t="n">
-        <v>8.93</v>
+        <v>37.67</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2074,29 +1866,29 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>New Hampshire</t>
+          <t>Texas -- Bexar County</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44103</v>
+        <v>44066</v>
       </c>
       <c r="C35" t="n">
-        <v>8233</v>
+        <v>45255</v>
       </c>
       <c r="D35" t="n">
-        <v>439</v>
+        <v>721</v>
       </c>
       <c r="E35" t="n">
-        <v>382</v>
+        <v>1329</v>
       </c>
       <c r="F35" t="n">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="G35" t="n">
-        <v>5.24</v>
+        <v>5.03</v>
       </c>
       <c r="H35" t="n">
-        <v>2.1</v>
+        <v>5.97</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
@@ -2105,16 +1897,16 @@
         <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>7285</v>
+        <v>26410</v>
       </c>
       <c r="L35" t="n">
-        <v>428</v>
+        <v>653</v>
       </c>
       <c r="M35" t="n">
-        <v>20516</v>
+        <v>146703</v>
       </c>
       <c r="N35" t="n">
-        <v>1.53</v>
+        <v>7.62</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2125,39 +1917,43 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44103</v>
+        <v>44104</v>
       </c>
       <c r="C36" t="n">
-        <v>29157</v>
+        <v>99134</v>
       </c>
       <c r="D36" t="n">
-        <v>875</v>
+        <v>2036</v>
       </c>
       <c r="E36" t="n">
-        <v>518</v>
-      </c>
-      <c r="F36" t="inlineStr"/>
+        <v>16920</v>
+      </c>
+      <c r="F36" t="n">
+        <v>195</v>
+      </c>
       <c r="G36" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="H36" t="inlineStr"/>
+        <v>17.07</v>
+      </c>
+      <c r="H36" t="n">
+        <v>9.58</v>
+      </c>
       <c r="I36" t="b">
         <v>1</v>
       </c>
       <c r="J36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="n">
-        <v>43006</v>
+        <v>342186</v>
       </c>
       <c r="N36" t="n">
-        <v>2.06</v>
+        <v>6.19</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2168,26 +1964,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>NewYork</t>
-        </is>
-      </c>
-      <c r="B37" s="2" t="n">
-        <v>44103</v>
-      </c>
-      <c r="C37" t="n">
-        <v>458649</v>
-      </c>
-      <c r="D37" t="n">
-        <v>25479</v>
-      </c>
+          <t>Nevada</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
-      <c r="F37" t="n">
-        <v>6454</v>
-      </c>
+      <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
-      <c r="H37" t="n">
-        <v>26.82</v>
-      </c>
+      <c r="H37" t="inlineStr"/>
       <c r="I37" t="b">
         <v>0</v>
       </c>
@@ -2195,65 +1981,59 @@
         <v>0</v>
       </c>
       <c r="K37" t="inlineStr"/>
-      <c r="L37" t="n">
-        <v>24061</v>
-      </c>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="n">
+        <v>261123</v>
+      </c>
+      <c r="N37" t="n">
+        <v>8.93</v>
+      </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>New York -- New York</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>239219</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>19187</t>
-        </is>
+        <v>44099</v>
+      </c>
+      <c r="C38" t="n">
+        <v>53607</v>
+      </c>
+      <c r="D38" t="n">
+        <v>15364</v>
       </c>
       <c r="E38" t="n">
-        <v>37274</v>
+        <v>8888</v>
       </c>
       <c r="F38" t="n">
-        <v>5345</v>
+        <v>1738</v>
       </c>
       <c r="G38" t="n">
-        <v>27.99</v>
+        <v>0.17</v>
       </c>
       <c r="H38" t="n">
-        <v>30.39</v>
+        <v>0.11</v>
       </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="b">
-        <v>1</v>
-      </c>
-      <c r="K38" t="n">
-        <v>133172</v>
-      </c>
-      <c r="L38" t="n">
-        <v>17586</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
       <c r="M38" t="n">
-        <v>2049418</v>
+        <v>3365783</v>
       </c>
       <c r="N38" t="n">
-        <v>24.27</v>
+        <v>12.07</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2264,58 +2044,40 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>North Carolina</t>
-        </is>
-      </c>
-      <c r="B39" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C39" t="n">
-        <v>210632</v>
-      </c>
-      <c r="D39" t="n">
-        <v>3532</v>
-      </c>
-      <c r="E39" t="n">
-        <v>38779</v>
-      </c>
-      <c r="F39" t="n">
-        <v>1014</v>
-      </c>
-      <c r="G39" t="n">
-        <v>23.26</v>
-      </c>
-      <c r="H39" t="n">
-        <v>30.14</v>
-      </c>
+          <t>Delaware</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39" t="b">
-        <v>1</v>
-      </c>
-      <c r="K39" t="n">
-        <v>166700</v>
-      </c>
-      <c r="L39" t="n">
-        <v>3364</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
       <c r="M39" t="n">
-        <v>2179622</v>
+        <v>209892</v>
       </c>
       <c r="N39" t="n">
-        <v>21.46</v>
+        <v>22.11</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>NorthDakota</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -2333,177 +2095,185 @@
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
+      <c r="M40" t="n">
+        <v>90860</v>
+      </c>
+      <c r="N40" t="n">
+        <v>4.77</v>
+      </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'text'")</t>
+          <t>An error occurred. ... KeyError('PositiveCases')</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Ohio</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>44103</v>
+      </c>
+      <c r="C41" t="n">
+        <v>810625</v>
+      </c>
+      <c r="D41" t="n">
+        <v>15792</v>
+      </c>
+      <c r="E41" t="n">
+        <v>24098</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1186</v>
+      </c>
+      <c r="G41" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="H41" t="n">
+        <v>7.64</v>
+      </c>
       <c r="I41" t="b">
         <v>0</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
       </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+      <c r="K41" t="n">
+        <v>564767</v>
+      </c>
+      <c r="L41" t="n">
+        <v>15516</v>
+      </c>
       <c r="M41" t="n">
-        <v>1438271</v>
+        <v>2267875</v>
       </c>
       <c r="N41" t="n">
-        <v>12.35</v>
+        <v>5.79</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>87199</v>
-      </c>
-      <c r="D42" t="n">
-        <v>1031</v>
-      </c>
-      <c r="E42" t="n">
-        <v>6226.008599999999</v>
-      </c>
-      <c r="F42" t="n">
-        <v>65.98399999999999</v>
-      </c>
-      <c r="G42" t="n">
-        <v>7.14</v>
-      </c>
-      <c r="H42" t="n">
-        <v>6.4</v>
-      </c>
+          <t>SouthDakota</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
       <c r="I42" t="b">
         <v>0</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
       </c>
-      <c r="K42" t="n">
-        <v>70814.3079</v>
-      </c>
-      <c r="L42" t="n">
-        <v>959.9641</v>
-      </c>
-      <c r="M42" t="n">
-        <v>287959</v>
-      </c>
-      <c r="N42" t="n">
-        <v>7.35</v>
-      </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Oregon</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+          <t>Vermont</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1752</v>
+      </c>
+      <c r="D43" t="n">
+        <v>58</v>
+      </c>
+      <c r="E43" t="n">
+        <v>174</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>10.26</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
       <c r="I43" t="b">
         <v>0</v>
       </c>
       <c r="J43" t="b">
-        <v>0</v>
-      </c>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K43" t="n">
+        <v>1696</v>
+      </c>
+      <c r="L43" t="n">
+        <v>58</v>
+      </c>
       <c r="M43" t="n">
-        <v>77789</v>
+        <v>8058</v>
       </c>
       <c r="N43" t="n">
-        <v>1.91</v>
+        <v>1.29</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>An error occurred. ... KeyError("None of ['Categories'] are in the columns")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C44" t="n">
-        <v>153924</v>
+        <v>29435</v>
       </c>
       <c r="D44" t="n">
-        <v>8142</v>
+        <v>877</v>
       </c>
       <c r="E44" t="n">
-        <v>20830</v>
-      </c>
-      <c r="F44" t="n">
-        <v>1668</v>
-      </c>
+        <v>521</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
-        <v>25.63</v>
-      </c>
-      <c r="H44" t="n">
-        <v>20.64</v>
-      </c>
+        <v>1.77</v>
+      </c>
+      <c r="H44" t="inlineStr"/>
       <c r="I44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="b">
-        <v>1</v>
-      </c>
-      <c r="K44" t="n">
-        <v>81282</v>
-      </c>
-      <c r="L44" t="n">
-        <v>8081</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
       <c r="M44" t="n">
-        <v>1423319</v>
+        <v>43006</v>
       </c>
       <c r="N44" t="n">
-        <v>11.13</v>
+        <v>2.06</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -2514,47 +2284,43 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Rhode Island</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>44015</v>
+        <v>44104</v>
       </c>
       <c r="C45" t="n">
-        <v>16491</v>
+        <v>698051</v>
       </c>
       <c r="D45" t="n">
-        <v>960</v>
+        <v>14315</v>
       </c>
       <c r="E45" t="n">
-        <v>1592</v>
+        <v>93993</v>
       </c>
       <c r="F45" t="n">
-        <v>48</v>
+        <v>2499</v>
       </c>
       <c r="G45" t="n">
-        <v>12.29</v>
+        <v>13.47</v>
       </c>
       <c r="H45" t="n">
-        <v>6.14</v>
+        <v>17.46</v>
       </c>
       <c r="I45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="b">
         <v>0</v>
       </c>
-      <c r="K45" t="n">
-        <v>12950</v>
-      </c>
-      <c r="L45" t="n">
-        <v>782</v>
-      </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
       <c r="M45" t="n">
-        <v>69254</v>
+        <v>3316376</v>
       </c>
       <c r="N45" t="n">
-        <v>6.55</v>
+        <v>16.1</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -2565,36 +2331,54 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SouthCarolina</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+          <t>Washington, DC</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C46" t="n">
+        <v>15326</v>
+      </c>
+      <c r="D46" t="n">
+        <v>627</v>
+      </c>
+      <c r="E46" t="n">
+        <v>7758</v>
+      </c>
+      <c r="F46" t="n">
+        <v>467</v>
+      </c>
+      <c r="G46" t="n">
+        <v>50.62</v>
+      </c>
+      <c r="H46" t="n">
+        <v>74.48</v>
+      </c>
       <c r="I46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
+      <c r="M46" t="n">
+        <v>321317</v>
+      </c>
+      <c r="N46" t="n">
+        <v>46.94</v>
+      </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'text'")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>SouthDakota</t>
+          <t>California - San Francisco</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -2616,50 +2400,54 @@
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C48" t="n">
-        <v>196139</v>
+        <v>70536</v>
       </c>
       <c r="D48" t="n">
-        <v>2454</v>
+        <v>2051</v>
       </c>
       <c r="E48" t="n">
-        <v>35639</v>
+        <v>2934</v>
       </c>
       <c r="F48" t="n">
-        <v>667</v>
+        <v>129</v>
       </c>
       <c r="G48" t="n">
-        <v>18.17</v>
+        <v>5.02</v>
       </c>
       <c r="H48" t="n">
-        <v>27.18</v>
+        <v>6.41</v>
       </c>
       <c r="I48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="b">
-        <v>1</v>
-      </c>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>58418</v>
+      </c>
+      <c r="L48" t="n">
+        <v>2013</v>
+      </c>
       <c r="M48" t="n">
-        <v>1117489</v>
+        <v>227938</v>
       </c>
       <c r="N48" t="n">
-        <v>16.8</v>
+        <v>4.12</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -2670,135 +2458,131 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Texas</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+          <t>California - San Diego</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C49" t="n">
+        <v>47180</v>
+      </c>
+      <c r="D49" t="n">
+        <v>783</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1725</v>
+      </c>
+      <c r="F49" t="n">
+        <v>33</v>
+      </c>
+      <c r="G49" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="H49" t="n">
+        <v>4.24</v>
+      </c>
       <c r="I49" t="b">
         <v>0</v>
       </c>
       <c r="J49" t="b">
         <v>0</v>
       </c>
-      <c r="K49" t="inlineStr"/>
-      <c r="L49" t="inlineStr"/>
+      <c r="K49" t="n">
+        <v>39060</v>
+      </c>
+      <c r="L49" t="n">
+        <v>779</v>
+      </c>
       <c r="M49" t="n">
-        <v>3365783</v>
+        <v>166412</v>
       </c>
       <c r="N49" t="n">
-        <v>12.07</v>
+        <v>5.04</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>An error occurred. ... XLRDError("No sheet named &lt;'Cases by RaceEthnicity'&gt;")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
-        </is>
-      </c>
-      <c r="B50" s="2" t="n">
-        <v>44066</v>
-      </c>
-      <c r="C50" t="n">
-        <v>45255</v>
-      </c>
-      <c r="D50" t="n">
-        <v>721</v>
-      </c>
-      <c r="E50" t="n">
-        <v>1329</v>
-      </c>
-      <c r="F50" t="n">
-        <v>39</v>
-      </c>
-      <c r="G50" t="n">
-        <v>5.03</v>
-      </c>
-      <c r="H50" t="n">
-        <v>5.97</v>
-      </c>
+          <t>Idaho</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
       <c r="I50" t="b">
         <v>0</v>
       </c>
       <c r="J50" t="b">
         <v>0</v>
       </c>
-      <c r="K50" t="n">
-        <v>26410</v>
-      </c>
-      <c r="L50" t="n">
-        <v>653</v>
-      </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
       <c r="M50" t="n">
-        <v>146703</v>
+        <v>11536</v>
       </c>
       <c r="N50" t="n">
-        <v>7.62</v>
+        <v>0.68</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
         <v>44104</v>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>73042</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>459</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>1473</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="C51" t="n">
+        <v>153924</v>
+      </c>
+      <c r="D51" t="n">
+        <v>8142</v>
+      </c>
+      <c r="E51" t="n">
+        <v>20830</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1668</v>
       </c>
       <c r="G51" t="n">
-        <v>2</v>
+        <v>25.63</v>
       </c>
       <c r="H51" t="n">
-        <v>1.53</v>
+        <v>20.64</v>
       </c>
       <c r="I51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="b">
-        <v>0</v>
-      </c>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K51" t="n">
+        <v>81282</v>
+      </c>
+      <c r="L51" t="n">
+        <v>8081</v>
+      </c>
       <c r="M51" t="n">
-        <v>35862</v>
+        <v>1423319</v>
       </c>
       <c r="N51" t="n">
-        <v>1.18</v>
+        <v>11.13</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -2809,94 +2593,76 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Vermont</t>
-        </is>
-      </c>
-      <c r="B52" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C52" t="n">
-        <v>1752</v>
-      </c>
-      <c r="D52" t="n">
-        <v>58</v>
-      </c>
-      <c r="E52" t="n">
-        <v>174</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="n">
-        <v>10.26</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0</v>
-      </c>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
       <c r="I52" t="b">
         <v>0</v>
       </c>
       <c r="J52" t="b">
-        <v>1</v>
-      </c>
-      <c r="K52" t="n">
-        <v>1696</v>
-      </c>
-      <c r="L52" t="n">
-        <v>58</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
       <c r="M52" t="n">
-        <v>8058</v>
+        <v>305259</v>
       </c>
       <c r="N52" t="n">
-        <v>1.29</v>
+        <v>4.39</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Virginia</t>
-        </is>
-      </c>
-      <c r="B53" s="3" t="n">
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C53" t="n">
-        <v>148254</v>
+        <v>318026</v>
       </c>
       <c r="D53" t="n">
-        <v>3208</v>
+        <v>7021</v>
       </c>
       <c r="E53" t="n">
-        <v>29679</v>
+        <v>84015</v>
       </c>
       <c r="F53" t="n">
-        <v>835</v>
+        <v>2881</v>
       </c>
       <c r="G53" t="n">
-        <v>20.02</v>
+        <v>26.42</v>
       </c>
       <c r="H53" t="n">
-        <v>26.03</v>
+        <v>41.03</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="n">
-        <v>1613285</v>
+        <v>3239300</v>
       </c>
       <c r="N53" t="n">
-        <v>19.17</v>
+        <v>31.46</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -2907,47 +2673,43 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Washington</t>
-        </is>
-      </c>
-      <c r="B54" s="2" t="n">
-        <v>44103</v>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="B54" s="3" t="n">
+        <v>44104</v>
       </c>
       <c r="C54" t="n">
-        <v>87042</v>
+        <v>148254</v>
       </c>
       <c r="D54" t="n">
-        <v>2124</v>
+        <v>3208</v>
       </c>
       <c r="E54" t="n">
-        <v>3499</v>
+        <v>29679</v>
       </c>
       <c r="F54" t="n">
-        <v>68</v>
+        <v>835</v>
       </c>
       <c r="G54" t="n">
-        <v>5.89</v>
+        <v>20.02</v>
       </c>
       <c r="H54" t="n">
-        <v>3.27</v>
+        <v>26.03</v>
       </c>
       <c r="I54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" t="b">
         <v>0</v>
       </c>
-      <c r="K54" t="n">
-        <v>59360</v>
-      </c>
-      <c r="L54" t="n">
-        <v>2081</v>
-      </c>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
       <c r="M54" t="n">
-        <v>269854</v>
+        <v>1613285</v>
       </c>
       <c r="N54" t="n">
-        <v>3.7</v>
+        <v>19.17</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -2958,174 +2720,156 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
-        </is>
-      </c>
-      <c r="B55" s="2" t="n">
-        <v>44104</v>
-      </c>
-      <c r="C55" t="n">
-        <v>15326</v>
-      </c>
-      <c r="D55" t="n">
-        <v>627</v>
-      </c>
-      <c r="E55" t="n">
-        <v>7758</v>
-      </c>
-      <c r="F55" t="n">
-        <v>467</v>
-      </c>
-      <c r="G55" t="n">
-        <v>50.62</v>
-      </c>
-      <c r="H55" t="n">
-        <v>74.48</v>
-      </c>
+          <t>WestVirginia</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
       <c r="I55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
-      <c r="M55" t="n">
-        <v>321317</v>
-      </c>
-      <c r="N55" t="n">
-        <v>46.94</v>
-      </c>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>WestVirginia</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C56" t="n">
+        <v>120019</v>
+      </c>
+      <c r="D56" t="n">
+        <v>3405</v>
+      </c>
+      <c r="E56" t="n">
+        <v>11545</v>
+      </c>
+      <c r="F56" t="n">
+        <v>449</v>
+      </c>
+      <c r="G56" t="n">
+        <v>9.619999999999999</v>
+      </c>
+      <c r="H56" t="n">
+        <v>13.19</v>
+      </c>
       <c r="I56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
+      <c r="M56" t="n">
+        <v>619472</v>
+      </c>
+      <c r="N56" t="n">
+        <v>9.33</v>
+      </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
-        </is>
-      </c>
-      <c r="B57" s="2" t="n">
-        <v>44090</v>
-      </c>
-      <c r="C57" t="n">
-        <v>91304</v>
-      </c>
-      <c r="D57" t="n">
-        <v>1220</v>
-      </c>
-      <c r="E57" t="n">
-        <v>10190</v>
-      </c>
-      <c r="F57" t="n">
-        <v>229</v>
-      </c>
-      <c r="G57" t="n">
-        <v>12.28</v>
-      </c>
-      <c r="H57" t="n">
-        <v>19.07</v>
-      </c>
+          <t>New Hampshire</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
       <c r="I57" t="b">
         <v>0</v>
       </c>
       <c r="J57" t="b">
-        <v>1</v>
-      </c>
-      <c r="K57" t="n">
-        <v>82991</v>
-      </c>
-      <c r="L57" t="n">
-        <v>1201</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
       <c r="M57" t="n">
-        <v>368744</v>
+        <v>20516</v>
       </c>
       <c r="N57" t="n">
-        <v>6.38</v>
+        <v>1.53</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B58" s="2" t="n">
         <v>44104</v>
       </c>
       <c r="C58" t="n">
-        <v>29054</v>
+        <v>68840</v>
       </c>
       <c r="D58" t="n">
-        <v>428</v>
+        <v>1174</v>
       </c>
       <c r="E58" t="n">
-        <v>7050</v>
+        <v>5604</v>
       </c>
       <c r="F58" t="n">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="G58" t="n">
-        <v>25.84</v>
+        <v>11.99</v>
       </c>
       <c r="H58" t="n">
-        <v>35.98</v>
+        <v>12.85</v>
       </c>
       <c r="I58" t="b">
         <v>0</v>
       </c>
       <c r="J58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58" t="n">
-        <v>27282</v>
+        <v>46742</v>
       </c>
       <c r="L58" t="n">
-        <v>428</v>
+        <v>1073</v>
       </c>
       <c r="M58" t="n">
-        <v>252321</v>
+        <v>354112</v>
       </c>
       <c r="N58" t="n">
-        <v>26.44</v>
+        <v>7.98</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -3136,33 +2880,51 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Wyoming</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
+          <t>California - Los Angeles</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>44103</v>
+      </c>
+      <c r="C59" t="n">
+        <v>270299</v>
+      </c>
+      <c r="D59" t="n">
+        <v>6576</v>
+      </c>
+      <c r="E59" t="n">
+        <v>7816</v>
+      </c>
+      <c r="F59" t="n">
+        <v>607</v>
+      </c>
+      <c r="G59" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="H59" t="n">
+        <v>9.81</v>
+      </c>
       <c r="I59" t="b">
         <v>0</v>
       </c>
       <c r="J59" t="b">
         <v>0</v>
       </c>
-      <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr"/>
+      <c r="K59" t="n">
+        <v>162023</v>
+      </c>
+      <c r="L59" t="n">
+        <v>6190</v>
+      </c>
       <c r="M59" t="n">
-        <v>5540</v>
+        <v>823987</v>
       </c>
       <c r="N59" t="n">
-        <v>0.95</v>
+        <v>8.16</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>An error occurred. ... KeyError('SUM(# probable)')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>